<commit_message>
Cambios en Documentacion y Reordenamiento del Repositorio
</commit_message>
<xml_diff>
--- a/Testing/Plan de Pruebas Integrales.xlsx
+++ b/Testing/Plan de Pruebas Integrales.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARCHIVOS\DATA SCIENCE\Repositorios\PROYECTO FINAL\PF-Esperanza-De-Vida\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C021A6-CBB1-4CF1-9233-C4C3436FC0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20F5FD2-D32F-4BEB-BB38-04646B9A5104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{38B65039-0485-42ED-9B8F-14BB8F65388E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Integrales SIN MLOps" sheetId="2" r:id="rId1"/>
-    <sheet name="Integrales CON MLOps" sheetId="3" r:id="rId2"/>
+    <sheet name="Integrales" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -111,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>ID DE PASO</t>
   </si>
@@ -257,12 +256,62 @@
   <si>
     <t>Link al Video</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SIN</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> MODELO DE MACHINE LEARNING IMPLEMENTADO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CON</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> MODELO DE MACHINE LEARNING IMPLEMENTADO</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,8 +385,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -356,8 +422,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -409,12 +487,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -453,6 +555,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -698,13 +818,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1257300</xdr:colOff>
-          <xdr:row>4</xdr:row>
+          <xdr:row>5</xdr:row>
           <xdr:rowOff>161925</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>2171700</xdr:colOff>
-          <xdr:row>4</xdr:row>
+          <xdr:row>5</xdr:row>
           <xdr:rowOff>847725</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -753,13 +873,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1228725</xdr:colOff>
-          <xdr:row>5</xdr:row>
+          <xdr:row>6</xdr:row>
           <xdr:rowOff>161925</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>2143125</xdr:colOff>
-          <xdr:row>5</xdr:row>
+          <xdr:row>6</xdr:row>
           <xdr:rowOff>847725</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1102,10 +1222,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C304C2A-776E-4326-9B5F-83418038D851}">
-  <dimension ref="A1:AF9"/>
+  <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,48 +1313,33 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:32" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>9</v>
-      </c>
+    <row r="5" spans="1:32" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:32" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="11">
+        <v>1</v>
+      </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="12"/>
+        <v>12</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="E6" s="5" t="s">
         <v>7</v>
       </c>
@@ -1242,7 +1347,7 @@
         <v>16</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="6" t="s">
@@ -1251,80 +1356,147 @@
       <c r="J6" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="AF6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:32" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
-        <v>2</v>
-      </c>
+      <c r="A7" s="11"/>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="F7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="5"/>
+      <c r="I7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="8" spans="1:32" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="5"/>
+    <row r="8" spans="1:32" s="15" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
+      <c r="AB8" s="14"/>
+      <c r="AC8" s="14"/>
+      <c r="AD8" s="14"/>
+      <c r="AE8" s="14"/>
+      <c r="AF8" s="14"/>
     </row>
     <row r="9" spans="1:32" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="11">
+        <v>2</v>
+      </c>
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="13"/>
+        <v>13</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="E9" s="5"/>
       <c r="F9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="5"/>
     </row>
+    <row r="10" spans="1:32" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:32" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
     <mergeCell ref="A1:J3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="A5:J5"/>
   </mergeCells>
-  <conditionalFormatting sqref="E5:E9">
+  <conditionalFormatting sqref="E6:E7 E9:E11">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"PENDIENTE"</formula>
     </cfRule>
@@ -1332,7 +1504,7 @@
       <formula>"FINALIZADO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5:J9">
+  <conditionalFormatting sqref="J6:J7 J9:J11">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"NO OK"</formula>
     </cfRule>
@@ -1341,13 +1513,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J9" xr:uid="{7AB34BB7-12DD-4646-B942-43CD4B334C3F}">
-      <formula1>$AF$4:$AF$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6:J7 J9:J11" xr:uid="{7AB34BB7-12DD-4646-B942-43CD4B334C3F}">
+      <formula1>$AF$4:$AF$6</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I5" r:id="rId1" xr:uid="{74391A81-F423-4F69-80BB-CB73363C9483}"/>
-    <hyperlink ref="I6" r:id="rId2" xr:uid="{9E2A33A2-411F-4403-B6D1-A909A21ADC38}"/>
+    <hyperlink ref="I6" r:id="rId1" xr:uid="{74391A81-F423-4F69-80BB-CB73363C9483}"/>
+    <hyperlink ref="I7" r:id="rId2" xr:uid="{9E2A33A2-411F-4403-B6D1-A909A21ADC38}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1362,13 +1534,13 @@
               <from>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>1257300</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>161925</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>2171700</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>847725</xdr:rowOff>
               </to>
             </anchor>
@@ -1387,13 +1559,13 @@
               <from>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>1228725</xdr:colOff>
-                <xdr:row>5</xdr:row>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>161925</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>2143125</xdr:colOff>
-                <xdr:row>5</xdr:row>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>847725</xdr:rowOff>
               </to>
             </anchor>
@@ -1406,16 +1578,4 @@
     </mc:AlternateContent>
   </oleObjects>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E06CD48-10B9-4777-B9BB-6B8F6F65642E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Pruebas integrales y funcion eliminar duplicados
</commit_message>
<xml_diff>
--- a/Testing/Plan de Pruebas Integrales.xlsx
+++ b/Testing/Plan de Pruebas Integrales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARCHIVOS\DATA SCIENCE\Repositorios\PROYECTO FINAL\PF-Esperanza-De-Vida\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20F5FD2-D32F-4BEB-BB38-04646B9A5104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56CAE62-B85B-48E6-95A3-5C492191F3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{38B65039-0485-42ED-9B8F-14BB8F65388E}"/>
   </bookViews>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>ID DE PASO</t>
   </si>
@@ -174,16 +174,6 @@
   <si>
     <t>CARGA INCREMENTAL
 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se Realizara una segunda carga de datos, teniendo datos en el DW por el paso anterior. Se trataran de novedades mas todos los datos del paso anterior. </t>
-  </si>
-  <si>
-    <t>CARGA INCREMENTAL
-3</t>
-  </si>
-  <si>
-    <t>Se Realizara una ultima carga de datos, teniendo datos en el DW por los dos pasos previos. Se trataran algunas modificaciones de datos existentes y datos repetidos. Solamente deberia realizar actualizaciones y no inserciones.</t>
   </si>
   <si>
     <r>
@@ -239,13 +229,7 @@
     </r>
   </si>
   <si>
-    <t>Se espera la carga parcial de los datos en el DW dado que ya hay registros presentes en big query. Ademas, seguramente el proceso realice algunas eliminaciones como parte del EDA e imputaciones de los datos nuevos a persistir.</t>
-  </si>
-  <si>
     <t>Se espera la carga de la totalidad de los datos en el DW, seguramente el proceso realice algunas eliminaciones como parte del EDA e imputaciones de los datos.</t>
-  </si>
-  <si>
-    <t>Se espera que el proceso solamente realice modificaciones de los registros que tengan diferencias. El resto deberia ignorarse por encontrarse persistidos en el DW.</t>
   </si>
   <si>
     <t>DATOS AUDITORIA</t>
@@ -305,6 +289,29 @@
       </rPr>
       <t xml:space="preserve"> MODELO DE MACHINE LEARNING IMPLEMENTADO</t>
     </r>
+  </si>
+  <si>
+    <t>Se Realizara una segunda carga de datos, teniendo datos en el DW por el paso anterior. Se trataran de novedades mas todos los datos del paso anterior. Se agregaran Registros Repetidos dentro de las Novedades.</t>
+  </si>
+  <si>
+    <t>Se espera la carga de la totalidad de los datos en el DW, seguramente el proceso realice algunas eliminaciones como parte del EDA e imputaciones de los datos.
+El Nro de Ejecucion en Auditoria es el 2. Se mantuvo la Ejecucion anterior en Auditoria para verificar que inserte la misma cantidad de Registros ya que lo que se hizo en esta prueba fue fraccionar los inputs/parametros.</t>
+  </si>
+  <si>
+    <t>Se espera la carga parcial de los datos en el DW dado que ya hay registros presentes en big query. Ademas, seguramente el proceso realice algunas eliminaciones como parte del EDA e imputaciones de los datos nuevos a persistir.
+El Nro de Ejecucion en Auditoria es el 3. Se mantuvo la Ejecucion anterior en Auditoria para verificar que inserte la misma cantidad de Registros ya que lo que se hizo en esta prueba fue fraccionar los inputs/parametros.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parametros_Paises.csv 
+Parametros_Indicadores.csv 
+Parametros_Indicador_Rentabilidad.csv 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+El Nro de Ejecucion en Auditoria es el 1 = Caso 1.1 
+El Nro de Ejecucion en Auditoria es el 2 = Caso 2.1
+El Nro de Ejecucion en Auditoria es el 3 = Caso 2.2</t>
   </si>
 </sst>
 </file>
@@ -435,7 +442,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -511,12 +518,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -535,6 +568,15 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -557,12 +599,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -574,6 +610,18 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -817,15 +865,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>1257300</xdr:colOff>
+          <xdr:colOff>1285875</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>590550</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>2171700</xdr:colOff>
+          <xdr:colOff>2200275</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>847725</xdr:rowOff>
+          <xdr:rowOff>1276350</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -872,15 +920,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>1228725</xdr:colOff>
+          <xdr:colOff>1209675</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>600075</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>2143125</xdr:colOff>
+          <xdr:colOff>2124075</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>847725</xdr:rowOff>
+          <xdr:rowOff>1285875</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -891,6 +939,721 @@
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>171450</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>752475</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1085850</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>1438275</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1031" name="Object 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1031"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1447800</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>742950</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>2362200</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>1428750</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1032" name="Object 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1032"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>2752725</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>733425</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>3667125</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>1419225</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1033" name="Object 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1033"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>228600</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>838200</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1143000</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>1524000</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1034" name="Object 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1034"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1504950</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>828675</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>2419350</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>1514475</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1035" name="Object 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1035"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>2809875</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>819150</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>3724275</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>1504950</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1036" name="Object 12" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1036"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>857250</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1190625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>1543050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1038" name="Object 14" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1038"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1524000</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>838200</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>2438400</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>1524000</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1039" name="Object 15" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1039"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>2838450</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>838200</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>3752850</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>1524000</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1040" name="Object 16" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1040"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>190500</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>847725</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1104900</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>1533525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1041" name="Object 17" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1041"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1514475</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>828675</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>2428875</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>1514475</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1042" name="Object 18" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1042"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>2828925</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>809625</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>3743325</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>1495425</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1043" name="Object 19" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1043"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>1285875</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>1943100</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>2200275</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>600075</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1045" name="Object 21" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1045"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1222,10 +1985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C304C2A-776E-4326-9B5F-83418038D851}">
-  <dimension ref="A1:AF11"/>
+  <dimension ref="A1:AF10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="I9" sqref="I9:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,9 +1996,9 @@
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.5703125" customWidth="1"/>
-    <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.85546875" customWidth="1"/>
+    <col min="6" max="6" width="60.7109375" customWidth="1"/>
     <col min="7" max="7" width="55.7109375" customWidth="1"/>
     <col min="8" max="8" width="53.42578125" customWidth="1"/>
     <col min="9" max="9" width="49" customWidth="1"/>
@@ -1243,40 +2006,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="A1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:32" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:32" ht="0.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1301,10 +2064,10 @@
         <v>1</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>3</v>
@@ -1314,21 +2077,21 @@
       </c>
     </row>
     <row r="5" spans="1:32" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
+      <c r="A5" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
     </row>
-    <row r="6" spans="1:32" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+    <row r="6" spans="1:32" ht="159.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1337,21 +2100,21 @@
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>23</v>
+      <c r="D6" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>16</v>
+      <c r="F6" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>8</v>
@@ -1360,19 +2123,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:32" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+    <row r="7" spans="1:32" ht="159.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="12"/>
+      <c r="D7" s="15"/>
       <c r="E7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="9" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1380,50 +2143,50 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:32" s="15" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="14"/>
-      <c r="Z8" s="14"/>
-      <c r="AA8" s="14"/>
-      <c r="AB8" s="14"/>
-      <c r="AC8" s="14"/>
-      <c r="AD8" s="14"/>
-      <c r="AE8" s="14"/>
-      <c r="AF8" s="14"/>
+    <row r="8" spans="1:32" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
     </row>
-    <row r="9" spans="1:32" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+    <row r="9" spans="1:32" ht="159.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1432,71 +2195,65 @@
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="1" t="s">
+      <c r="D9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="10" spans="1:32" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+    <row r="10" spans="1:32" ht="159.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>16</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:32" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="H10" s="22"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="A1:J3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="D9:D10"/>
     <mergeCell ref="A8:J8"/>
     <mergeCell ref="A5:J5"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
   </mergeCells>
-  <conditionalFormatting sqref="E6:E7 E9:E11">
+  <conditionalFormatting sqref="E6:E7 E9:E10">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"PENDIENTE"</formula>
     </cfRule>
@@ -1504,7 +2261,7 @@
       <formula>"FINALIZADO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J6:J7 J9:J11">
+  <conditionalFormatting sqref="J6:J7 J9:J10">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"NO OK"</formula>
     </cfRule>
@@ -1513,67 +2270,393 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6:J7 J9:J11" xr:uid="{7AB34BB7-12DD-4646-B942-43CD4B334C3F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6:J7 J9:J10" xr:uid="{7AB34BB7-12DD-4646-B942-43CD4B334C3F}">
       <formula1>$AF$4:$AF$6</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="I6" r:id="rId1" xr:uid="{74391A81-F423-4F69-80BB-CB73363C9483}"/>
     <hyperlink ref="I7" r:id="rId2" xr:uid="{9E2A33A2-411F-4403-B6D1-A909A21ADC38}"/>
+    <hyperlink ref="I9:I10" r:id="rId3" display="Link al Video" xr:uid="{B73A43CA-291D-43ED-B8B2-8D4EF55B5A96}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Worksheet" dvAspect="DVASPECT_ICON" shapeId="1027" r:id="rId6">
-          <objectPr defaultSize="0" r:id="rId7">
+        <oleObject progId="Worksheet" dvAspect="DVASPECT_ICON" shapeId="1027" r:id="rId7">
+          <objectPr defaultSize="0" r:id="rId8">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>7</xdr:col>
-                <xdr:colOff>1257300</xdr:colOff>
+                <xdr:colOff>1285875</xdr:colOff>
                 <xdr:row>5</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
+                <xdr:rowOff>590550</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
-                <xdr:colOff>2171700</xdr:colOff>
+                <xdr:colOff>2200275</xdr:colOff>
                 <xdr:row>5</xdr:row>
-                <xdr:rowOff>847725</xdr:rowOff>
+                <xdr:rowOff>1276350</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Worksheet" dvAspect="DVASPECT_ICON" shapeId="1027" r:id="rId6"/>
+        <oleObject progId="Worksheet" dvAspect="DVASPECT_ICON" shapeId="1027" r:id="rId7"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Worksheet" dvAspect="DVASPECT_ICON" shapeId="1028" r:id="rId8">
-          <objectPr defaultSize="0" r:id="rId9">
+        <oleObject progId="Worksheet" dvAspect="DVASPECT_ICON" shapeId="1028" r:id="rId9">
+          <objectPr defaultSize="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>7</xdr:col>
-                <xdr:colOff>1228725</xdr:colOff>
+                <xdr:colOff>1209675</xdr:colOff>
                 <xdr:row>6</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
+                <xdr:rowOff>600075</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
-                <xdr:colOff>2143125</xdr:colOff>
+                <xdr:colOff>2124075</xdr:colOff>
                 <xdr:row>6</xdr:row>
-                <xdr:rowOff>847725</xdr:rowOff>
+                <xdr:rowOff>1285875</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Worksheet" dvAspect="DVASPECT_ICON" shapeId="1028" r:id="rId8"/>
+        <oleObject progId="Worksheet" dvAspect="DVASPECT_ICON" shapeId="1028" r:id="rId9"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1031" r:id="rId11">
+          <objectPr defaultSize="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>171450</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>752475</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1085850</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>1438275</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1031" r:id="rId11"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1032" r:id="rId13">
+          <objectPr defaultSize="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1447800</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>742950</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>2362200</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>1428750</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1032" r:id="rId13"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1033" r:id="rId15">
+          <objectPr defaultSize="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>2752725</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>733425</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>3667125</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>1419225</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1033" r:id="rId15"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1034" r:id="rId17">
+          <objectPr defaultSize="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>838200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1143000</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>1524000</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1034" r:id="rId17"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1035" r:id="rId18">
+          <objectPr defaultSize="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1504950</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>828675</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>2419350</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>1514475</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1035" r:id="rId18"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1036" r:id="rId19">
+          <objectPr defaultSize="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>2809875</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>819150</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>3724275</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>1504950</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1036" r:id="rId19"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1038" r:id="rId20">
+          <objectPr defaultSize="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>276225</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>857250</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1190625</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>1543050</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1038" r:id="rId20"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1039" r:id="rId22">
+          <objectPr defaultSize="0" r:id="rId23">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1524000</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>838200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>2438400</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>1524000</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1039" r:id="rId22"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1040" r:id="rId24">
+          <objectPr defaultSize="0" r:id="rId25">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>2838450</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>838200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>3752850</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>1524000</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1040" r:id="rId24"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1041" r:id="rId26">
+          <objectPr defaultSize="0" r:id="rId27">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>190500</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>847725</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1104900</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>1533525</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1041" r:id="rId26"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1042" r:id="rId28">
+          <objectPr defaultSize="0" r:id="rId29">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1514475</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>828675</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>2428875</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>1514475</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1042" r:id="rId28"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1043" r:id="rId30">
+          <objectPr defaultSize="0" r:id="rId31">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>2828925</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>809625</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>3743325</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>1495425</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Macro-Enabled Worksheet" dvAspect="DVASPECT_ICON" shapeId="1043" r:id="rId30"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Worksheet" dvAspect="DVASPECT_ICON" shapeId="1045" r:id="rId32">
+          <objectPr defaultSize="0" r:id="rId33">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>1285875</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>1943100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>2200275</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>600075</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Worksheet" dvAspect="DVASPECT_ICON" shapeId="1045" r:id="rId32"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>

</xml_diff>